<commit_message>
data and graphical update
</commit_message>
<xml_diff>
--- a/data/candidemia-data.xlsx
+++ b/data/candidemia-data.xlsx
@@ -8,30 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\WORK\CEMA\MAP-AMR\Dashboard\appdir\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C7C23A-A6F4-4BBA-9064-4D78F41150DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4296BF-761B-4FC0-81D8-819C6B4C6F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="2040" windowWidth="17280" windowHeight="10500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="2040" windowWidth="17280" windowHeight="10500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="KNH" sheetId="1" r:id="rId1"/>
-    <sheet name="KNH-summary" sheetId="11" r:id="rId2"/>
-    <sheet name="KNH-candida" sheetId="12" r:id="rId3"/>
-    <sheet name="Totals" sheetId="10" r:id="rId4"/>
+    <sheet name="Totals" sheetId="10" r:id="rId1"/>
+    <sheet name="KNH" sheetId="1" r:id="rId2"/>
+    <sheet name="KNH-summary" sheetId="11" r:id="rId3"/>
+    <sheet name="KNH-candida" sheetId="12" r:id="rId4"/>
     <sheet name="TNH" sheetId="2" r:id="rId5"/>
-    <sheet name="CGTRH" sheetId="3" r:id="rId6"/>
-    <sheet name="JOOTRH" sheetId="4" r:id="rId7"/>
-    <sheet name="Machakos level 5" sheetId="5" r:id="rId8"/>
-    <sheet name="MPShah" sheetId="6" r:id="rId9"/>
-    <sheet name="KUTRRH" sheetId="7" r:id="rId10"/>
-    <sheet name="AKUH" sheetId="8" r:id="rId11"/>
-    <sheet name="CVC tips" sheetId="9" r:id="rId12"/>
+    <sheet name="TNH-summary" sheetId="13" r:id="rId6"/>
+    <sheet name="TNH-candida" sheetId="14" r:id="rId7"/>
+    <sheet name="CGTRH" sheetId="3" r:id="rId8"/>
+    <sheet name="JOOTRH" sheetId="4" r:id="rId9"/>
+    <sheet name="Machakos level 5" sheetId="5" r:id="rId10"/>
+    <sheet name="MPShah" sheetId="6" r:id="rId11"/>
+    <sheet name="KUTRRH" sheetId="7" r:id="rId12"/>
+    <sheet name="AKUH" sheetId="8" r:id="rId13"/>
+    <sheet name="CVC tips" sheetId="9" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="231">
   <si>
     <t>Month</t>
   </si>
@@ -1274,6 +1276,918 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C333F6-233F-4794-AC4C-2CDB93138D57}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="18" max="18" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="9" max="9" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" customWidth="1"/>
+    <col min="12" max="12" width="23.77734375" customWidth="1"/>
+    <col min="13" max="13" width="60.109375" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="24.44140625" customWidth="1"/>
+    <col min="18" max="18" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="13">
+        <v>10485310</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="62">
+        <v>45566</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="62">
+        <v>45597</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="62">
+        <v>45330</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13">
+        <v>10554075</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="61">
+        <v>45394</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" customWidth="1"/>
+    <col min="13" max="13" width="62.88671875" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+    <col min="18" max="18" width="16.21875" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="13">
+        <v>62</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="61">
+        <v>45355</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="61">
+        <v>45359</v>
+      </c>
+      <c r="K2" s="61">
+        <v>45364</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>24043818</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="26.21875" customWidth="1"/>
+    <col min="14" max="14" width="23" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1000041524</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="13">
+        <v>4</v>
+      </c>
+      <c r="I2" s="61">
+        <v>45328</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="K2" s="61">
+        <v>45350</v>
+      </c>
+      <c r="L2" s="61">
+        <v>45353</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2" s="61">
+        <v>45411</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="61">
+        <v>45358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1000762907</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1</v>
+      </c>
+      <c r="I3" s="61">
+        <v>45302</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="K3" s="61">
+        <v>45351</v>
+      </c>
+      <c r="L3" s="61">
+        <v>45353</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q3" s="61">
+        <v>45411</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="61">
+        <v>45367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="13">
+        <v>10212423</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="13">
+        <v>5</v>
+      </c>
+      <c r="I4" s="61">
+        <v>45333</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="61">
+        <v>45343</v>
+      </c>
+      <c r="L4" s="61">
+        <v>45346</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q4" s="61">
+        <v>45415</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="61">
+        <v>45349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="13">
+        <v>10354355</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="13">
+        <v>6</v>
+      </c>
+      <c r="I5" s="61">
+        <v>45304</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="61">
+        <v>45336</v>
+      </c>
+      <c r="L5" s="61">
+        <v>45339</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q5" s="61">
+        <v>45415</v>
+      </c>
+      <c r="S5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="61">
+        <v>45341</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="W1:AB1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5696,572 +6610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" customWidth="1"/>
-    <col min="13" max="13" width="62.88671875" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" customWidth="1"/>
-    <col min="18" max="18" width="16.21875" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" s="13">
-        <v>62</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="H2" s="61">
-        <v>45355</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="J2" s="61">
-        <v>45359</v>
-      </c>
-      <c r="K2" s="61">
-        <v>45364</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q2" s="13">
-        <v>24043818</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>188</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AB5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="9" max="9" width="19.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="20.88671875" customWidth="1"/>
-    <col min="12" max="12" width="17.109375" customWidth="1"/>
-    <col min="13" max="13" width="26.21875" customWidth="1"/>
-    <col min="14" max="14" width="23" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="63" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="13">
-        <v>1000041524</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="13">
-        <v>4</v>
-      </c>
-      <c r="I2" s="61">
-        <v>45328</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="K2" s="61">
-        <v>45350</v>
-      </c>
-      <c r="L2" s="61">
-        <v>45353</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q2" s="61">
-        <v>45411</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="61">
-        <v>45358</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="13">
-        <v>1000762907</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="13">
-        <v>1</v>
-      </c>
-      <c r="I3" s="61">
-        <v>45302</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="K3" s="61">
-        <v>45351</v>
-      </c>
-      <c r="L3" s="61">
-        <v>45353</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q3" s="61">
-        <v>45411</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="61">
-        <v>45367</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28">
-      <c r="A4" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="13">
-        <v>10212423</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" s="13">
-        <v>5</v>
-      </c>
-      <c r="I4" s="61">
-        <v>45333</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="61">
-        <v>45343</v>
-      </c>
-      <c r="L4" s="61">
-        <v>45346</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q4" s="61">
-        <v>45415</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="T4" s="61">
-        <v>45349</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28">
-      <c r="A5" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="13">
-        <v>10354355</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="13">
-        <v>6</v>
-      </c>
-      <c r="I5" s="61">
-        <v>45304</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="K5" s="61">
-        <v>45336</v>
-      </c>
-      <c r="L5" s="61">
-        <v>45339</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="P5" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q5" s="61">
-        <v>45415</v>
-      </c>
-      <c r="S5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="61">
-        <v>45341</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="W1:AB1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D6E28F-FC04-49B2-83C9-1E88376F113E}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -6445,12 +6794,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E6D978-5361-455B-9648-CC9751D4AA66}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -6497,75 +6846,6 @@
       </c>
       <c r="B5">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C333F6-233F-4794-AC4C-2CDB93138D57}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>216</v>
-      </c>
-      <c r="B7">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -16590,6 +16870,247 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541746E-CC5A-4B4A-9CCB-391BD8B560C2}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>65</v>
+      </c>
+      <c r="F2">
+        <v>71</v>
+      </c>
+      <c r="G2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>74</v>
+      </c>
+      <c r="E3">
+        <v>81</v>
+      </c>
+      <c r="F3">
+        <v>92</v>
+      </c>
+      <c r="G3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>74</v>
+      </c>
+      <c r="F4">
+        <v>72</v>
+      </c>
+      <c r="G4">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C70568F-8036-4DFA-BB63-2ECD11B5985F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16669,7 +17190,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -16772,282 +17293,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:S1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="18" max="18" width="15.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:S3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="9" max="9" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
-    <col min="12" max="12" width="23.77734375" customWidth="1"/>
-    <col min="13" max="13" width="60.109375" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="24.44140625" customWidth="1"/>
-    <col min="18" max="18" width="14.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="13">
-        <v>10485310</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="62">
-        <v>45566</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J2" s="62">
-        <v>45597</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="62">
-        <v>45330</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="13">
-        <v>10554075</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="J3" s="61">
-        <v>45394</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>